<commit_message>
IDM ready for test set creation
</commit_message>
<xml_diff>
--- a/HW6/Documentation/PDF-Submission/IDM.xlsx
+++ b/HW6/Documentation/PDF-Submission/IDM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\SE-4367-Testing\HW6\Documentation\PDF-Submission\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BB2067-3562-467B-8346-60C8D2554145}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3941925D-7CC7-4FA9-88D2-FD695FEE44BF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{14BDEA4B-8CFD-4AEA-8261-4DB328586FC1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
   <si>
     <t>Fact</t>
   </si>
@@ -120,18 +120,12 @@
     <t>a new value and a null value</t>
   </si>
   <si>
-    <t>Step4</t>
-  </si>
-  <si>
     <t>This is where BCC comes into play</t>
   </si>
   <si>
     <t>Author</t>
   </si>
   <si>
-    <t>Base Choice</t>
-  </si>
-  <si>
     <t>The model is base choice</t>
   </si>
   <si>
@@ -147,12 +141,6 @@
     <t>Test Set</t>
   </si>
   <si>
-    <t xml:space="preserve">Slide </t>
-  </si>
-  <si>
-    <t>Slide 25</t>
-  </si>
-  <si>
     <t>Choosing combinations</t>
   </si>
   <si>
@@ -166,6 +154,36 @@
   </si>
   <si>
     <t>facts.xml</t>
+  </si>
+  <si>
+    <t>Step 4</t>
+  </si>
+  <si>
+    <t>Fact IDM</t>
+  </si>
+  <si>
+    <t>Fact Base Choice</t>
+  </si>
+  <si>
+    <t>Slide 31</t>
+  </si>
+  <si>
+    <t>Slide 18+ 31</t>
+  </si>
+  <si>
+    <t>Slide 18</t>
+  </si>
+  <si>
+    <t>Slide 11-33</t>
+  </si>
+  <si>
+    <t>Documentation of Reasonsing</t>
+  </si>
+  <si>
+    <t>The test set is…</t>
+  </si>
+  <si>
+    <t>I chose this because…</t>
   </si>
 </sst>
 </file>
@@ -315,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -360,6 +378,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -674,36 +693,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD443C5D-124B-4746-B604-C7241A91ECD7}">
-  <dimension ref="C2:K26"/>
+  <dimension ref="B1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="6" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="6" width="14.85546875" customWidth="1"/>
     <col min="7" max="7" width="14.140625" customWidth="1"/>
     <col min="9" max="9" width="12.28515625" style="7" customWidth="1"/>
     <col min="10" max="10" width="47.140625" style="7" customWidth="1"/>
     <col min="11" max="11" width="9.140625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J1" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="12" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
-      <c r="I2" s="8" t="s">
+    </row>
+    <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
@@ -716,8 +738,14 @@
       <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I3" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
@@ -730,12 +758,8 @@
       <c r="F4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="9"/>
-    </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
@@ -748,14 +772,12 @@
       <c r="F5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I5" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="9"/>
+    </row>
+    <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="6" t="s">
         <v>6</v>
       </c>
@@ -768,111 +790,141 @@
       <c r="F6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="21"/>
-      <c r="J6" s="11" t="s">
+      <c r="I6" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="I7" s="22" t="s">
+    <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="I8" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J8" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I8" s="20" t="s">
+    <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="I9" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J9" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="18"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="11" t="s">
+    <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C10" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C11" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="I11" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="J11" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="I11" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="20"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="I12" s="20" t="s">
+        <v>48</v>
+      </c>
       <c r="J12" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
       <c r="I13" s="20"/>
       <c r="J13" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I14" s="20"/>
+      <c r="J14" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I14" s="21"/>
-      <c r="J14" s="11" t="s">
+    <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="18"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="18"/>
-      <c r="I15" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="J15" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C16" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D16" s="16"/>
-      <c r="I16" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="J16" s="10" t="s">
-        <v>32</v>
+      <c r="I16" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.25">
@@ -880,9 +932,11 @@
         <v>5</v>
       </c>
       <c r="D17" s="17"/>
-      <c r="I17" s="20"/>
+      <c r="I17" s="20" t="s">
+        <v>46</v>
+      </c>
       <c r="J17" s="10" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -892,44 +946,60 @@
       <c r="D18" s="6"/>
       <c r="I18" s="20"/>
       <c r="J18" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.25">
       <c r="I19" s="20"/>
       <c r="J19" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I20" s="21"/>
-      <c r="J20" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="J22" s="7" t="s">
-        <v>14</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I20" s="20"/>
+      <c r="J20" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I21" s="21"/>
+      <c r="J21" s="11" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="3:10" x14ac:dyDescent="0.25">
       <c r="J23" s="7" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="J24" s="23" t="s">
-        <v>44</v>
+      <c r="J24" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="3:10" x14ac:dyDescent="0.25">
       <c r="J25" s="23" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="3:10" x14ac:dyDescent="0.25">
       <c r="J26" s="23" t="s">
-        <v>46</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J27" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J29" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J31" s="7" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>